<commit_message>
Update metabolome_limma_analysis (from correct script) (with separated metabolites with 2HMDBs) 5.xlsx
</commit_message>
<xml_diff>
--- a/R analysis of metabolome data/Results/metabolome_limma_analysis (from correct script) (with separated metabolites with 2HMDBs) 5.xlsx
+++ b/R analysis of metabolome data/Results/metabolome_limma_analysis (from correct script) (with separated metabolites with 2HMDBs) 5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabde\OneDrive\Documents\UM documents\BMS Year 3\Internship + Thesis\Sabrina_BMS_Bachelor-Internship\R analysis of metabolome data\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96759593-44D7-483B-B50B-4E48898C7988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF8D199-BBF5-4D82-A0DD-032EF6C54887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="0" windowWidth="9360" windowHeight="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metabolome_limma_analysis (from" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="297">
   <si>
     <t>logFC</t>
   </si>
@@ -121,9 +121,6 @@
     <t>HMDB00574</t>
   </si>
   <si>
-    <t>HMDB02994|HMDB04136</t>
-  </si>
-  <si>
     <t>HMDB00251</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>HMDB00725</t>
   </si>
   <si>
-    <t>HMDB00172|HMDB00687</t>
-  </si>
-  <si>
     <t>HMDB00622</t>
   </si>
   <si>
@@ -295,9 +289,6 @@
     <t>HMDB0000243</t>
   </si>
   <si>
-    <t>HMDB00039|HMDB01873</t>
-  </si>
-  <si>
     <t>HMDB02329</t>
   </si>
   <si>
@@ -325,9 +316,6 @@
     <t>HMDB00779</t>
   </si>
   <si>
-    <t>HMDB11756|HMDB61684</t>
-  </si>
-  <si>
     <t>HMDB60015</t>
   </si>
   <si>
@@ -635,9 +623,6 @@
   </si>
   <si>
     <t>HMDB00824</t>
-  </si>
-  <si>
-    <t>HMDB28783|HMDB29014|</t>
   </si>
   <si>
     <t>HMDB06695</t>
@@ -1832,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G329"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A149" sqref="A149"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2280,7 +2265,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B20">
         <v>-4972809.1930803498</v>
@@ -2303,7 +2288,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B21">
         <v>195016.22250446401</v>
@@ -2326,7 +2311,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B22">
         <v>155536.259321786</v>
@@ -2349,7 +2334,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B23">
         <v>-49086.481474107102</v>
@@ -2372,7 +2357,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B24">
         <v>-58286.576900624998</v>
@@ -2395,7 +2380,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B25">
         <v>-54248.875159374998</v>
@@ -2418,7 +2403,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26">
         <v>12988.1251102232</v>
@@ -2441,7 +2426,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B27">
         <v>-10572.5715888839</v>
@@ -2464,7 +2449,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B28">
         <v>-249566.25777</v>
@@ -2487,7 +2472,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B29">
         <v>-6580988.5944642797</v>
@@ -2510,7 +2495,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B30">
         <v>-11766.602013080301</v>
@@ -2533,7 +2518,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B31">
         <v>24885.990832767799</v>
@@ -2579,7 +2564,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B33">
         <v>42671.085631696398</v>
@@ -2602,7 +2587,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B34">
         <v>-8189.1584741964298</v>
@@ -2625,7 +2610,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B35">
         <v>61466.802980357097</v>
@@ -2648,7 +2633,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B36">
         <v>-45179.743856785703</v>
@@ -2671,7 +2656,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B37">
         <v>247792.48375892799</v>
@@ -2694,7 +2679,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B38">
         <v>31153.453279017798</v>
@@ -2717,7 +2702,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B39">
         <v>697332.95091071201</v>
@@ -2740,7 +2725,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B40">
         <v>-51217.995325669603</v>
@@ -2763,7 +2748,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B41">
         <v>-377295.77335714299</v>
@@ -2786,7 +2771,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B42">
         <v>671734.83208526694</v>
@@ -2809,7 +2794,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B43">
         <v>7175.5814971428499</v>
@@ -2832,7 +2817,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B44">
         <v>141311.95136830301</v>
@@ -2855,7 +2840,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B45">
         <v>628982.62712499895</v>
@@ -2878,7 +2863,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B46">
         <v>-212410.36884375001</v>
@@ -2901,7 +2886,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B47">
         <v>-460587.23639446398</v>
@@ -2924,7 +2909,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B48">
         <v>994317.514484821</v>
@@ -2947,7 +2932,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B49">
         <v>138419.97139107101</v>
@@ -2970,7 +2955,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B50">
         <v>345167.05444343702</v>
@@ -2993,7 +2978,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B51">
         <v>101096.22688482099</v>
@@ -3016,7 +3001,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B52">
         <v>20973.639106651801</v>
@@ -3039,7 +3024,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B53">
         <v>-174739.26530089299</v>
@@ -3062,7 +3047,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B54">
         <v>-93777.803428571497</v>
@@ -3085,7 +3070,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B55">
         <v>176610.24704330301</v>
@@ -3108,7 +3093,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B56">
         <v>22485.797364732101</v>
@@ -3131,7 +3116,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B57">
         <v>-40199.5834833482</v>
@@ -3154,7 +3139,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B58">
         <v>16731.159231875001</v>
@@ -3177,7 +3162,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B59">
         <v>-18836.580404017899</v>
@@ -3200,7 +3185,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B60">
         <v>649800.76877678395</v>
@@ -3223,7 +3208,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B61">
         <v>-118661.393248928</v>
@@ -3246,7 +3231,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B62">
         <v>386918.77899107098</v>
@@ -3269,7 +3254,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B63">
         <v>1011988.38495535</v>
@@ -3292,7 +3277,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B64">
         <v>-109961.17960334801</v>
@@ -3315,7 +3300,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B65">
         <v>524185.83349107002</v>
@@ -3338,7 +3323,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B66">
         <v>-6613.07253360714</v>
@@ -3361,7 +3346,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B67">
         <v>57006.630465624898</v>
@@ -3384,7 +3369,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B68">
         <v>29941.534997589199</v>
@@ -3407,7 +3392,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B69">
         <v>133694.793508929</v>
@@ -3430,7 +3415,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B70">
         <v>612050.36310714297</v>
@@ -3453,7 +3438,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B71">
         <v>930608.21273124998</v>
@@ -3476,7 +3461,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B72">
         <v>27501.699084821401</v>
@@ -3499,7 +3484,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B73">
         <v>42067.426755357097</v>
@@ -3522,7 +3507,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B74">
         <v>-36625.487341071399</v>
@@ -3568,7 +3553,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B76">
         <v>4369.1801539999897</v>
@@ -3591,7 +3576,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B77">
         <v>-334709.76537455298</v>
@@ -3614,7 +3599,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B78">
         <v>19929.608802901799</v>
@@ -3637,7 +3622,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B79">
         <v>-1003132.4304017799</v>
@@ -3660,7 +3645,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B80">
         <v>-11471.235334687501</v>
@@ -3683,7 +3668,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B81">
         <v>569236.77710223105</v>
@@ -3706,7 +3691,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B82">
         <v>-39215.600745133903</v>
@@ -3729,7 +3714,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B83">
         <v>3560056.9698258899</v>
@@ -3752,7 +3737,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B84">
         <v>-14319.0965514286</v>
@@ -3775,7 +3760,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B85">
         <v>156145.14471785701</v>
@@ -3798,7 +3783,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B86">
         <v>-17730.213635089302</v>
@@ -3821,7 +3806,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B87">
         <v>-2601.3714403214299</v>
@@ -3844,7 +3829,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B88">
         <v>-95676.374843303507</v>
@@ -3867,7 +3852,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B89">
         <v>555856.88750267902</v>
@@ -3890,7 +3875,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B90">
         <v>-14985.5177236607</v>
@@ -3913,7 +3898,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B91">
         <v>704294.68292857101</v>
@@ -3936,7 +3921,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B92">
         <v>-90258.244116071393</v>
@@ -3959,7 +3944,7 @@
     </row>
     <row r="93" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B93" s="7">
         <v>-109079.572233884</v>
@@ -3982,7 +3967,7 @@
     </row>
     <row r="94" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="6" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B94" s="7">
         <v>-109079.572233884</v>
@@ -4005,7 +3990,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B95">
         <v>366899.62568169599</v>
@@ -4028,7 +4013,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B96">
         <v>1927661.9099330299</v>
@@ -4051,7 +4036,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B97">
         <v>-3368.5666571294601</v>
@@ -4074,7 +4059,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B98">
         <v>17374.960422812499</v>
@@ -4097,7 +4082,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B99">
         <v>-17391.344688883899</v>
@@ -4120,7 +4105,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B100">
         <v>90970.3466249997</v>
@@ -4143,7 +4128,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B101">
         <v>-3437.4606541294602</v>
@@ -4166,7 +4151,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B102">
         <v>84963.245039553498</v>
@@ -4189,7 +4174,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B103">
         <v>-145476.230133929</v>
@@ -4212,7 +4197,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B104">
         <v>-27152.310612053599</v>
@@ -4235,7 +4220,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B105">
         <v>756708.40522321395</v>
@@ -4258,7 +4243,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B106">
         <v>178644.08256607101</v>
@@ -4281,7 +4266,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B107">
         <v>89201.723447321303</v>
@@ -4304,7 +4289,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B108">
         <v>279033.04353124899</v>
@@ -4327,7 +4312,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B109">
         <v>9113.6934725892697</v>
@@ -4350,7 +4335,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B110">
         <v>-34484.897870892797</v>
@@ -4373,7 +4358,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B111">
         <v>35485.3590207589</v>
@@ -4396,7 +4381,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B112">
         <v>-2103.6359658035699</v>
@@ -4419,7 +4404,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B113">
         <v>52144.199090624898</v>
@@ -4442,7 +4427,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B114">
         <v>-2069261.0041308</v>
@@ -4465,7 +4450,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B115">
         <v>14391.384938158</v>
@@ -4488,7 +4473,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B116">
         <v>648048.676825893</v>
@@ -4511,7 +4496,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B117">
         <v>-1830465.7292191901</v>
@@ -4534,7 +4519,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B118">
         <v>1398562.6915424101</v>
@@ -4557,7 +4542,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B119">
         <v>2618839.7979017799</v>
@@ -4580,7 +4565,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B120">
         <v>-29352.243278124901</v>
@@ -4603,7 +4588,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B121">
         <v>66532.883036607105</v>
@@ -4626,7 +4611,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B122">
         <v>54641.567380357003</v>
@@ -4649,7 +4634,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B123">
         <v>37654.031349374898</v>
@@ -4672,7 +4657,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B124">
         <v>-129199.995549107</v>
@@ -4695,7 +4680,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B125">
         <v>34965.6578950892</v>
@@ -4718,7 +4703,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B126">
         <v>-23858.838522633901</v>
@@ -4741,7 +4726,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B127">
         <v>-6207.8268900982102</v>
@@ -4764,7 +4749,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B128">
         <v>8132.11397142855</v>
@@ -4787,7 +4772,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B129">
         <v>49507.105939374902</v>
@@ -4810,7 +4795,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B130">
         <v>796283.39687991096</v>
@@ -4833,7 +4818,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B131">
         <v>60967.200563660699</v>
@@ -4856,7 +4841,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B132">
         <v>-204012.78012589301</v>
@@ -4879,7 +4864,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B133">
         <v>-25376.828283705399</v>
@@ -4902,7 +4887,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B134">
         <v>-148071.164347768</v>
@@ -4925,7 +4910,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B135">
         <v>121873.444594196</v>
@@ -4948,7 +4933,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B136">
         <v>1040561.64578571</v>
@@ -4971,7 +4956,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B137">
         <v>-50425.707892857099</v>
@@ -4994,7 +4979,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B138">
         <v>26475.676840624899</v>
@@ -5017,7 +5002,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B139">
         <v>-10898.035696875</v>
@@ -5040,7 +5025,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B140">
         <v>-4056.5076230803502</v>
@@ -5063,7 +5048,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B141">
         <v>-42541.614677232203</v>
@@ -5086,7 +5071,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B142">
         <v>1631776.8007589299</v>
@@ -5109,7 +5094,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B143">
         <v>11795.698161607101</v>
@@ -5132,7 +5117,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B144">
         <v>5115.98552433035</v>
@@ -5155,7 +5140,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B145">
         <v>-98559.673690625001</v>
@@ -5178,7 +5163,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B146">
         <v>4976.70623379463</v>
@@ -5224,7 +5209,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B148">
         <v>-1394355.06131339</v>
@@ -5247,7 +5232,7 @@
     </row>
     <row r="149" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A149" s="6" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B149" s="7">
         <v>246763.07602231999</v>
@@ -5270,7 +5255,7 @@
     </row>
     <row r="150" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A150" s="6" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B150" s="7">
         <v>246763.07602231999</v>
@@ -5293,7 +5278,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A151" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B151">
         <v>-22855.2409309375</v>
@@ -5316,7 +5301,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A152" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B152">
         <v>29892.4514112053</v>
@@ -5339,7 +5324,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A153" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B153">
         <v>-4358.3399629464302</v>
@@ -5362,7 +5347,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A154" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B154">
         <v>206095.868155134</v>
@@ -5385,7 +5370,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A155" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B155">
         <v>-4067.1059479687501</v>
@@ -5408,7 +5393,7 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A156" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B156">
         <v>-12585.226877499999</v>
@@ -5431,7 +5416,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A157" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B157">
         <v>6242.5270349330303</v>
@@ -5454,7 +5439,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A158" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B158">
         <v>-2366.4881653571301</v>
@@ -5477,7 +5462,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A159" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B159">
         <v>245736.480872321</v>
@@ -5500,7 +5485,7 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A160" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B160">
         <v>12733.3095721428</v>
@@ -5523,7 +5508,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A161" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B161">
         <v>318870.460108036</v>
@@ -5546,7 +5531,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A162" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B162">
         <v>-872017.12130714301</v>
@@ -5569,7 +5554,7 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A163" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B163">
         <v>351196.94994196302</v>
@@ -5592,7 +5577,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A164" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B164">
         <v>56581.997479062396</v>
@@ -5615,7 +5600,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A165" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B165">
         <v>-45766.633782589299</v>
@@ -5638,7 +5623,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A166" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B166">
         <v>-308636.81921294599</v>
@@ -5661,7 +5646,7 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A167" s="3" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B167">
         <v>-41403.556946205303</v>
@@ -5684,7 +5669,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A168" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B168">
         <v>3926.8532934526702</v>
@@ -5707,7 +5692,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A169" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B169">
         <v>79578.606624553504</v>
@@ -5730,7 +5715,7 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A170" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B170">
         <v>21340.4691977232</v>
@@ -5753,7 +5738,7 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A171" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B171">
         <v>93825.209825446305</v>
@@ -5799,7 +5784,7 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A173" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B173">
         <v>-51654.103356473199</v>
@@ -5822,7 +5807,7 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A174" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B174">
         <v>91500.888322321305</v>
@@ -5845,7 +5830,7 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A175" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B175">
         <v>89218.983105803403</v>
@@ -5868,7 +5853,7 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A176" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B176">
         <v>-10386.260358437499</v>
@@ -5891,7 +5876,7 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A177" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B177">
         <v>2922.3339547410601</v>
@@ -5914,7 +5899,7 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A178" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B178">
         <v>14071.508098660701</v>
@@ -5937,7 +5922,7 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A179" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B179">
         <v>-23861.606526785799</v>
@@ -5960,7 +5945,7 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A180" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B180">
         <v>17588.210944196398</v>
@@ -5983,7 +5968,7 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A181" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B181">
         <v>115447.61940312501</v>
@@ -6006,7 +5991,7 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A182" s="3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B182">
         <v>22696.113630026801</v>
@@ -6029,7 +6014,7 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A183" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B183">
         <v>2312.7020174999998</v>
@@ -6052,7 +6037,7 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A184" s="3" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B184">
         <v>3187406.4179464201</v>
@@ -6075,7 +6060,7 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A185" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B185">
         <v>126583.397197321</v>
@@ -6098,7 +6083,7 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A186" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B186">
         <v>5135.5894689732004</v>
@@ -6121,7 +6106,7 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A187" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B187">
         <v>290561.86911714298</v>
@@ -6144,7 +6129,7 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A188" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B188">
         <v>-45879.664474553603</v>
@@ -6167,7 +6152,7 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A189" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B189">
         <v>-2072801.7465580399</v>
@@ -6190,7 +6175,7 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A190" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B190">
         <v>193340.25767410701</v>
@@ -6213,7 +6198,7 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A191" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B191">
         <v>278562.63338973199</v>
@@ -6236,7 +6221,7 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A192" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B192">
         <v>495183.45669598202</v>
@@ -6259,7 +6244,7 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A193" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B193">
         <v>-256364.78776785699</v>
@@ -6282,7 +6267,7 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A194" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B194">
         <v>165302.54198660699</v>
@@ -6305,7 +6290,7 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A195" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B195">
         <v>207841.764366071</v>
@@ -6328,7 +6313,7 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A196" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B196">
         <v>3034527.0277285702</v>
@@ -6351,7 +6336,7 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A197" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B197">
         <v>-7519.5632280357104</v>
@@ -6374,7 +6359,7 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A198" s="3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B198">
         <v>162764.924700893</v>
@@ -6397,7 +6382,7 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A199" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B199">
         <v>2531.6011038839301</v>
@@ -6420,7 +6405,7 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A200" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B200">
         <v>2835.5454248660699</v>
@@ -6443,7 +6428,7 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A201" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B201">
         <v>735890.21982142795</v>
@@ -6466,7 +6451,7 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A202" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B202">
         <v>40268.710612365998</v>
@@ -6489,7 +6474,7 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A203" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B203">
         <v>-6617.3415273660703</v>
@@ -6512,7 +6497,7 @@
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A204" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B204">
         <v>63656.598791517798</v>
@@ -6535,7 +6520,7 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A205" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B205">
         <v>29315.953689285601</v>
@@ -6581,7 +6566,7 @@
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A207" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B207">
         <v>1137868.48120535</v>
@@ -6604,7 +6589,7 @@
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A208" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B208">
         <v>-61267.762160714199</v>
@@ -6650,7 +6635,7 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A210" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B210">
         <v>3865.2113908035599</v>
@@ -6673,7 +6658,7 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A211" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B211">
         <v>-2427.2091437500098</v>
@@ -6696,7 +6681,7 @@
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A212" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B212">
         <v>-227821.02605803599</v>
@@ -6719,7 +6704,7 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A213" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B213">
         <v>-175160.57816785699</v>
@@ -6765,7 +6750,7 @@
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A215" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B215">
         <v>7617.9920102678298</v>
@@ -6788,7 +6773,7 @@
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A216" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B216">
         <v>1922.7066107232099</v>
@@ -6811,7 +6796,7 @@
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A217" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B217">
         <v>-6954.9192766964297</v>
@@ -6834,7 +6819,7 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A218" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B218">
         <v>-1170967.0931696401</v>
@@ -6857,7 +6842,7 @@
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A219" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B219">
         <v>796.07427384375001</v>
@@ -6880,7 +6865,7 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A220" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B220">
         <v>1785.4687328125001</v>
@@ -6926,7 +6911,7 @@
     </row>
     <row r="222" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A222" s="6" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B222" s="7">
         <v>-3606.82443986607</v>
@@ -6949,7 +6934,7 @@
     </row>
     <row r="223" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A223" s="6" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B223" s="7">
         <v>-3606.82443986607</v>
@@ -6972,7 +6957,7 @@
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A224" s="3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B224">
         <v>1073.566138125</v>
@@ -6995,7 +6980,7 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A225" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B225">
         <v>-650787.91128124995</v>
@@ -7018,7 +7003,7 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A226" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B226">
         <v>183360.38495745501</v>
@@ -7041,7 +7026,7 @@
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A227" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B227">
         <v>-103129.053875</v>
@@ -7064,7 +7049,7 @@
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A228" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B228">
         <v>-1560.06410589286</v>
@@ -7087,7 +7072,7 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A229" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B229">
         <v>65566.197925446395</v>
@@ -7110,7 +7095,7 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A230" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B230">
         <v>23260.377896875001</v>
@@ -7133,7 +7118,7 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A231" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B231">
         <v>-899.27303888392601</v>
@@ -7156,7 +7141,7 @@
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A232" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B232">
         <v>-158288.957571429</v>
@@ -7179,7 +7164,7 @@
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A233" s="3" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B233">
         <v>-15432.692736160699</v>
@@ -7202,7 +7187,7 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A234" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B234">
         <v>27123.561613392802</v>
@@ -7225,7 +7210,7 @@
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A235" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B235">
         <v>-45084.914674553598</v>
@@ -7248,7 +7233,7 @@
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A236" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B236">
         <v>5367.9361423035698</v>
@@ -7271,7 +7256,7 @@
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A237" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B237">
         <v>7725.4766830357103</v>
@@ -7294,7 +7279,7 @@
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A238" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B238">
         <v>8689.7787980535704</v>
@@ -7340,7 +7325,7 @@
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A240" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B240">
         <v>1319.9715347410699</v>
@@ -7363,7 +7348,7 @@
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A241" s="3" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B241">
         <v>-79341.4741160712</v>
@@ -7386,7 +7371,7 @@
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A242" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B242">
         <v>-2757.6553095535901</v>
@@ -7409,7 +7394,7 @@
     </row>
     <row r="243" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A243" s="6" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B243" s="7">
         <v>-42921.9606236607</v>
@@ -7432,7 +7417,7 @@
     </row>
     <row r="244" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A244" s="6" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B244" s="7">
         <v>-42921.9606236607</v>
@@ -7455,7 +7440,7 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A245" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B245">
         <v>3129.64267125892</v>
@@ -7478,7 +7463,7 @@
     </row>
     <row r="246" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A246" s="8" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B246" s="7">
         <v>215670.06054910601</v>
@@ -7501,7 +7486,7 @@
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A247" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B247">
         <v>3444.77235321428</v>
@@ -7524,7 +7509,7 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A248" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B248">
         <v>-28600.1800790179</v>
@@ -7547,7 +7532,7 @@
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A249" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B249">
         <v>17049.5717981249</v>
@@ -7570,7 +7555,7 @@
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A250" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B250">
         <v>-197238.62119642799</v>
@@ -7593,7 +7578,7 @@
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A251" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B251">
         <v>-5126.4504283035703</v>
@@ -7616,7 +7601,7 @@
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A252" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B252">
         <v>-6310.9880080356897</v>
@@ -7639,7 +7624,7 @@
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A253" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B253">
         <v>-4736.12171415179</v>
@@ -7662,7 +7647,7 @@
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A254" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B254">
         <v>3149.4431092856998</v>
@@ -7685,7 +7670,7 @@
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A255" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B255">
         <v>-1353.93330901339</v>
@@ -7708,7 +7693,7 @@
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A256" s="3" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B256">
         <v>44488.663629910698</v>
@@ -7731,7 +7716,7 @@
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A257" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B257">
         <v>-35019.157944642997</v>
@@ -7754,7 +7739,7 @@
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A258" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B258">
         <v>550.07625308035597</v>
@@ -7777,7 +7762,7 @@
     </row>
     <row r="259" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A259" s="8" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B259" s="7">
         <v>3877.37209999997</v>
@@ -7800,7 +7785,7 @@
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A260" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B260">
         <v>124512.060317589</v>
@@ -7823,7 +7808,7 @@
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A261" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B261">
         <v>1169.7035968749899</v>
@@ -7846,7 +7831,7 @@
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A262" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B262">
         <v>-962.36638892857502</v>
@@ -7869,7 +7854,7 @@
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A263" s="3" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B263">
         <v>2054.3749697008898</v>
@@ -7892,7 +7877,7 @@
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A264" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B264">
         <v>1139.2646397767801</v>
@@ -7915,7 +7900,7 @@
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A265" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B265">
         <v>-100785.16604375</v>
@@ -7938,7 +7923,7 @@
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A266" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B266">
         <v>10207.5521643303</v>
@@ -7984,7 +7969,7 @@
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A268" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B268">
         <v>8023.4900572321103</v>
@@ -8007,7 +7992,7 @@
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A269" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B269">
         <v>-9621.6045545892703</v>
@@ -8030,7 +8015,7 @@
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A270" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B270">
         <v>6634.3084339732104</v>
@@ -8053,7 +8038,7 @@
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A271" s="3" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B271">
         <v>-34212.648459821401</v>
@@ -8076,7 +8061,7 @@
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A272" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B272">
         <v>-561.18314174107297</v>
@@ -8099,7 +8084,7 @@
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A273" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B273">
         <v>3869.6451450892901</v>
@@ -8122,7 +8107,7 @@
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A274" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B274">
         <v>-40156.6283705358</v>
@@ -8145,7 +8130,7 @@
     </row>
     <row r="275" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A275" s="6" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B275" s="7">
         <v>-413.56567567857201</v>
@@ -8168,7 +8153,7 @@
     </row>
     <row r="276" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A276" s="6" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B276" s="7">
         <v>-413.56567567857201</v>
@@ -8191,7 +8176,7 @@
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A277" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B277">
         <v>52641.5457973214</v>
@@ -8214,7 +8199,7 @@
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A278" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B278">
         <v>4046.8128229464101</v>
@@ -8237,7 +8222,7 @@
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A279" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B279">
         <v>651.71820656249497</v>
@@ -8260,7 +8245,7 @@
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A280" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B280">
         <v>42324.840115178697</v>
@@ -8283,7 +8268,7 @@
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A281" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B281">
         <v>4247.2802387499996</v>
@@ -8306,7 +8291,7 @@
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A282" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B282">
         <v>1182.008167</v>
@@ -8329,7 +8314,7 @@
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A283" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B283">
         <v>29487.220163995498</v>
@@ -8352,7 +8337,7 @@
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A284" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B284">
         <v>-16971.1215504465</v>
@@ -8375,7 +8360,7 @@
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A285" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B285">
         <v>-13248.6060862053</v>
@@ -8398,7 +8383,7 @@
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A286" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B286">
         <v>903.63025718749702</v>
@@ -8421,7 +8406,7 @@
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A287" s="3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B287">
         <v>-63145.193778571498</v>
@@ -8444,7 +8429,7 @@
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A288" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B288">
         <v>-3267.6078587946499</v>
@@ -8467,7 +8452,7 @@
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A289" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B289">
         <v>2742.1075405803499</v>
@@ -8490,7 +8475,7 @@
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A290" s="3" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B290">
         <v>-6867.8972562499903</v>
@@ -8513,7 +8498,7 @@
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A291" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B291">
         <v>-2688.3657802232201</v>
@@ -8536,7 +8521,7 @@
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A292" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B292">
         <v>-62524.109616071502</v>
@@ -8559,7 +8544,7 @@
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A293" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B293">
         <v>-913.64738808035395</v>
@@ -8582,7 +8567,7 @@
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A294" s="3" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B294">
         <v>81854.400062499801</v>
@@ -8605,7 +8590,7 @@
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A295" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B295">
         <v>-664.32451227679201</v>
@@ -8628,7 +8613,7 @@
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A296" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B296">
         <v>-13993.542069107099</v>
@@ -8651,7 +8636,7 @@
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A297" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B297">
         <v>1072.8147196428599</v>
@@ -8674,7 +8659,7 @@
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A298" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B298">
         <v>-19159.646763393201</v>
@@ -8697,7 +8682,7 @@
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A299" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B299">
         <v>-65039.234200892097</v>
@@ -8720,7 +8705,7 @@
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A300" s="3" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B300">
         <v>-619973.34040178603</v>
@@ -8743,7 +8728,7 @@
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A301" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B301">
         <v>-5197.8963594196503</v>
@@ -8766,7 +8751,7 @@
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A302" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B302">
         <v>6009.5055239731701</v>
@@ -8789,7 +8774,7 @@
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A303" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B303">
         <v>-291.88980092857201</v>
@@ -8812,7 +8797,7 @@
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A304" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B304">
         <v>75209.886410714505</v>
@@ -8835,7 +8820,7 @@
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A305" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B305">
         <v>9521.6169865624906</v>
@@ -8858,7 +8843,7 @@
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A306" s="3" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B306">
         <v>-89020.169700892802</v>
@@ -8881,7 +8866,7 @@
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A307" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B307">
         <v>187636.65446901799</v>
@@ -8927,7 +8912,7 @@
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A309" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B309">
         <v>-3003.3580193749699</v>
@@ -8950,7 +8935,7 @@
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A310" s="3" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B310">
         <v>-56623.447803571602</v>
@@ -8973,7 +8958,7 @@
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A311" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B311">
         <v>-2441.7577085267899</v>
@@ -8996,7 +8981,7 @@
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A312" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B312">
         <v>2408.31682857139</v>
@@ -9042,7 +9027,7 @@
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A314" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B314">
         <v>-22918.745378839201</v>
@@ -9065,7 +9050,7 @@
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A315" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B315">
         <v>6432.0451308034799</v>
@@ -9088,7 +9073,7 @@
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A316" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B316">
         <v>-965.76896558035901</v>
@@ -9111,7 +9096,7 @@
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A317" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B317">
         <v>1421.7248374553401</v>
@@ -9134,7 +9119,7 @@
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A318" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B318">
         <v>10105.457501339501</v>
@@ -9157,7 +9142,7 @@
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A319" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B319">
         <v>-671.37135812501504</v>
@@ -9180,7 +9165,7 @@
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A320" s="3" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B320">
         <v>53702.183839284502</v>
@@ -9203,7 +9188,7 @@
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A321" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B321">
         <v>-634.983983290173</v>
@@ -9226,7 +9211,7 @@
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A322" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B322">
         <v>558.97974782142398</v>
@@ -9249,7 +9234,7 @@
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A323" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B323">
         <v>64.435438392857193</v>
@@ -9272,7 +9257,7 @@
     </row>
     <row r="324" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A324" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B324">
         <v>2307.8917683035402</v>
@@ -9295,7 +9280,7 @@
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A325" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B325">
         <v>-193.839989196451</v>
@@ -9318,7 +9303,7 @@
     </row>
     <row r="326" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A326" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B326">
         <v>71.638605669635496</v>
@@ -9341,7 +9326,7 @@
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A327" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B327">
         <v>34.538754866069397</v>
@@ -9364,7 +9349,7 @@
     </row>
     <row r="328" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A328" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B328">
         <v>-1655.2691339282001</v>
@@ -9387,7 +9372,7 @@
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A329" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B329">
         <v>-1005.61427232157</v>

</xml_diff>